<commit_message>
#462 엑셀 업로드를 통한 상품수집 개선 https://ones.cn/project/#/team/YEhe758P/task/App17VwP86qQQ7BH
</commit_message>
<xml_diff>
--- a/public/sampleFile/exclPrdUpload.xlsx
+++ b/public/sampleFile/exclPrdUpload.xlsx
@@ -27,9 +27,124 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>상품URL</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>상품URL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>（필수 입력）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>상품명</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(최대 50자, 미입력시 자동 번역된 상품명 적용)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>키워드</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(카테고리 자동 추천)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>배송비</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(숫자만 입력 가능,예:10000)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>상품태그</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(최대 20개,콤마로 구분,띄어쓰기는 자동 삭제)</t>
+    </r>
+  </si>
+  <si>
+    <t>메모</t>
   </si>
 </sst>
 </file>
@@ -42,8 +157,16 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
-    <font>
+  <fonts count="21">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -521,142 +644,154 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1183,21 +1318,47 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="70.25" customWidth="1"/>
+    <col min="1" max="1" width="58.75" customWidth="1"/>
+    <col min="2" max="2" width="53.875" customWidth="1"/>
+    <col min="3" max="3" width="27.25" customWidth="1"/>
+    <col min="4" max="4" width="34.25" style="1" customWidth="1"/>
+    <col min="5" max="5" width="55" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="4:4">
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="4:4">
+      <c r="D3" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>